<commit_message>
database design to workbench database - 24.06.2023
</commit_message>
<xml_diff>
--- a/JAVA18 QPHAN DATABASE DESIGN.xlsx
+++ b/JAVA18 QPHAN DATABASE DESIGN.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="422" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="422" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="B1. Mô hình quan niệm" sheetId="1" r:id="rId1"/>
     <sheet name="B2. Mô hình logic" sheetId="2" r:id="rId2"/>
+    <sheet name="B3. Mô hình quan hệ" sheetId="3" r:id="rId3"/>
+    <sheet name="4. Cơ sở dữ liệu vật lý" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -354,8 +357,235 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="W4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+thuộc tính đa trị</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Đã đặt hàng, đang đóng gói, đang giao, giao thành công, giao thất bại</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+varchar || char
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+varchar</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Số lượng còn lại</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Số lượng còn lại</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+thuộc tính đơn trị</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+1 - N</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+1 - N</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="142">
   <si>
     <t>Xác định các đối tượng cần lưu trữ
 Xác định các thuộc tính, thông tin của từng đối tượng</t>
@@ -642,13 +872,324 @@
   </si>
   <si>
     <t>T12</t>
+  </si>
+  <si>
+    <t>1. Xác định các bảng</t>
+  </si>
+  <si>
+    <t>2. Xác định lại các thuộc tính(đơn) của từng bảng</t>
+  </si>
+  <si>
+    <t>3. Xác định khóa chính</t>
+  </si>
+  <si>
+    <t>4. Xử lý các mối quan hệ --&gt; khóa ngoại(11, 1n), bảng mới(NN)</t>
+  </si>
+  <si>
+    <t>Khóa chính</t>
+  </si>
+  <si>
+    <t>Khóa ngoại</t>
+  </si>
+  <si>
+    <t>Khóa chính - ngoại</t>
+  </si>
+  <si>
+    <t>ITEM_DETAIL</t>
+  </si>
+  <si>
+    <t>ITEM_ID</t>
+  </si>
+  <si>
+    <t>SIZE_ID</t>
+  </si>
+  <si>
+    <t>COLOR</t>
+  </si>
+  <si>
+    <t>ITEM_GROUP_ID</t>
+  </si>
+  <si>
+    <t>PROVIDER_ID</t>
+  </si>
+  <si>
+    <t>EMPLOYEE_DETAIL</t>
+  </si>
+  <si>
+    <t>EMPLOYEE_ID</t>
+  </si>
+  <si>
+    <t>TITLE_ID</t>
+  </si>
+  <si>
+    <t>Phụ Cấp</t>
+  </si>
+  <si>
+    <t>CUSTOMER_ID</t>
+  </si>
+  <si>
+    <t>ORDER_DETAIL</t>
+  </si>
+  <si>
+    <t>ORDER_ID</t>
+  </si>
+  <si>
+    <t>PAYMENT_METHOD_ID</t>
+  </si>
+  <si>
+    <t>DEPARTMENT_ID</t>
+  </si>
+  <si>
+    <t>ORDER_DELIVERY_STATUS_DETAIL</t>
+  </si>
+  <si>
+    <t>STATUS_ID</t>
+  </si>
+  <si>
+    <t>T13</t>
+  </si>
+  <si>
+    <t>T14</t>
+  </si>
+  <si>
+    <t>T15</t>
+  </si>
+  <si>
+    <t>T16</t>
+  </si>
+  <si>
+    <t>Sau khi thiết kết xong cơ sở dữ liệu(mô hình quan hệ) ở bước 3</t>
+  </si>
+  <si>
+    <t>Có 2 cách để tạo ra cơ sở dữ liệu vật lý nằm trong chương trình(MySQL workbench) của hệ quản trị cơ sở dữ liệu(MySQL)</t>
+  </si>
+  <si>
+    <t>DML: Data Manipulation Language: INSERT/DELETE/UPDATE/SELECT</t>
+  </si>
+  <si>
+    <t>DDL: CREATE/ALTER/DROP DATABASE, TABLE, CONSTRAINT, FUNCTION, PROCEDURE, VIEW ==&gt; structure, cấu trúc của cơ sở dữ liệu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lưu ý 1: Tạo bảng cha(1) trước --&gt; bảng con(N), thêm ràng buộc khóa ngoại đến bản cha(1) </t>
+  </si>
+  <si>
+    <t>Lưu ý 2: Tạo ra tất cả các bảng tùy ý --&gt; xem mối quan hệ để tạo ra ràng buộc khóa ngoại</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Thực tế:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Quản lý theo phiên bản</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Thực tế:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Tạo bảng cha(riêng lẻ) trước, những cụm chứa bảng cha, con có quan hệ với nhau được tạo ra 1 lần --&gt; tạo từng patchset</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(sql file)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> để tạo ra DB object cũng như lưu trữ code tạo DB</t>
+    </r>
+  </si>
+  <si>
+    <t>Thực tế: Quá trình quản lý phiên bản cho database --&gt; hỗ trợ cho việc migration</t>
+  </si>
+  <si>
+    <t>B1. Tạo ra ERD - diagram có structure của mô hình quan hệ ở bước 3 : File --&gt; New Model --&gt; Add Diagram</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B2: Từ diagram chuyển đổi sang SQL - DDL : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Database --&gt; Forward Engineer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> --&gt; Lưu nội dung code SQL DDL lại  (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Diagram --&gt; SQL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nếu muốn xem diagram: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Database --&gt; Reverse Engineer (SQL --&gt; Diagram)</t>
+    </r>
+  </si>
+  <si>
+    <t>B3. Kết nối vào account(connection) của HQT CSDL --&gt; mở file sql ddl --&gt; thực thi --&gt; cở sở dữ liệu</t>
+  </si>
+  <si>
+    <t>Thuận lợi: Tạo nhanh 1 cơ sở dữ liệu, dễ hình dung, kéo thả tự sinh ra khóa ngoại, bảng mới khi có quan hệ 1-N, 1-1, NN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hạn chế 1: Khó quản lý patchset, sql version </t>
+  </si>
+  <si>
+    <t>Hạn chế 2: Khi thay đổi database structure, nếu reverse eng --&gt; thay đổi --&gt; forward eng(ddl) --&gt; mất dữ liệu cũ</t>
+  </si>
+  <si>
+    <t>Khuyến khích: Lần 1 --&gt; tạo digram hoàn chỉnh --&gt; nếu có sai thì dùng code tay để chỉnh sửa, lưu phiên bản</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cách 1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Sử dụng </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SQL - DDL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Data Definition Language) code tay các dòng lệnh để tạo ra từng TABLE, COLUMN, CONSTRAINT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cách 2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Sử dụng TOOL - MySQL workbench</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -700,6 +1241,36 @@
     <font>
       <sz val="18"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -764,7 +1335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -802,18 +1373,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -835,6 +1397,49 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -850,6 +1455,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>712304</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>273325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1825486</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>287481</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2228021" y="11314042"/>
+          <a:ext cx="10058400" cy="7733548"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1145,16 +1799,16 @@
       </c>
     </row>
     <row r="2" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
     </row>
     <row r="3" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
       <c r="E3" s="7" t="s">
         <v>5</v>
       </c>
@@ -1163,9 +1817,9 @@
       </c>
     </row>
     <row r="4" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
       <c r="E4" s="7" t="s">
         <v>6</v>
       </c>
@@ -1552,8 +2206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
@@ -1580,16 +2234,16 @@
       </c>
     </row>
     <row r="2" spans="2:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
     </row>
     <row r="3" spans="2:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
       <c r="E3" s="7" t="s">
         <v>5</v>
       </c>
@@ -1598,9 +2252,9 @@
       </c>
     </row>
     <row r="4" spans="2:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
       <c r="E4" s="7" t="s">
         <v>6</v>
       </c>
@@ -1669,13 +2323,13 @@
       <c r="P5" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="Q5" s="21" t="s">
+      <c r="Q5" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="R5" s="22" t="s">
+      <c r="R5" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="S5" s="23" t="s">
+      <c r="S5" s="20" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1718,40 +2372,40 @@
       </c>
     </row>
     <row r="7" spans="2:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="J7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="L7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="M7" s="19" t="s">
+      <c r="M7" s="16" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1789,10 +2443,10 @@
       <c r="L8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="M8" s="19" t="s">
+      <c r="M8" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="Q8" s="21"/>
+      <c r="Q8" s="18"/>
     </row>
     <row r="9" spans="2:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
@@ -1865,10 +2519,10 @@
       <c r="P10" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="Q10" s="21" t="s">
+      <c r="Q10" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="R10" s="22" t="s">
+      <c r="R10" s="19" t="s">
         <v>63</v>
       </c>
       <c r="S10" s="7" t="s">
@@ -1909,7 +2563,7 @@
       <c r="M11" s="3"/>
     </row>
     <row r="12" spans="2:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="17" t="s">
         <v>80</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1931,7 +2585,7 @@
       <c r="M12" s="3"/>
     </row>
     <row r="13" spans="2:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="17" t="s">
         <v>81</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1951,7 +2605,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
-      <c r="Q13" s="24" t="s">
+      <c r="Q13" s="21" t="s">
         <v>75</v>
       </c>
       <c r="S13" s="7" t="s">
@@ -1985,10 +2639,10 @@
       <c r="P14" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="Q14" s="21" t="s">
+      <c r="Q14" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="R14" s="22" t="s">
+      <c r="R14" s="19" t="s">
         <v>63</v>
       </c>
       <c r="S14" s="7" t="s">
@@ -2020,10 +2674,10 @@
       <c r="P15" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="Q15" s="21" t="s">
+      <c r="Q15" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="R15" s="22" t="s">
+      <c r="R15" s="19" t="s">
         <v>63</v>
       </c>
       <c r="S15" s="7" t="s">
@@ -2054,10 +2708,10 @@
       <c r="P16" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="Q16" s="21" t="s">
+      <c r="Q16" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="R16" s="22" t="s">
+      <c r="R16" s="19" t="s">
         <v>63</v>
       </c>
       <c r="S16" s="7" t="s">
@@ -2087,10 +2741,10 @@
       <c r="P17" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="Q17" s="21" t="s">
+      <c r="Q17" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="R17" s="22" t="s">
+      <c r="R17" s="19" t="s">
         <v>63</v>
       </c>
       <c r="S17" s="7" t="s">
@@ -2135,20 +2789,20 @@
       </c>
     </row>
     <row r="21" spans="1:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
       <c r="P21" s="7" t="s">
         <v>77</v>
       </c>
@@ -2157,18 +2811,18 @@
       </c>
     </row>
     <row r="22" spans="1:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="18"/>
-      <c r="B22" s="15" t="s">
+      <c r="A22" s="38"/>
+      <c r="B22" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
       <c r="P22" s="7" t="s">
         <v>64</v>
       </c>
@@ -2177,17 +2831,17 @@
       </c>
     </row>
     <row r="23" spans="1:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="15"/>
-      <c r="C23" s="15" t="s">
+      <c r="B23" s="13"/>
+      <c r="C23" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
       <c r="P23" s="7" t="s">
         <v>69</v>
       </c>
@@ -2196,17 +2850,17 @@
       </c>
     </row>
     <row r="24" spans="1:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
       <c r="P24" s="7" t="s">
         <v>70</v>
       </c>
@@ -2215,17 +2869,17 @@
       </c>
     </row>
     <row r="25" spans="1:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="17" t="s">
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="H25" s="15"/>
+      <c r="H25" s="13"/>
       <c r="P25" s="7" t="s">
         <v>71</v>
       </c>
@@ -2234,15 +2888,15 @@
       </c>
     </row>
     <row r="26" spans="1:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="15"/>
-      <c r="C26" s="15" t="s">
+      <c r="B26" s="13"/>
+      <c r="C26" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
       <c r="P26" s="7" t="s">
         <v>79</v>
       </c>
@@ -2282,6 +2936,998 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" style="7" customWidth="1"/>
+    <col min="2" max="3" width="30.7109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="32.85546875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" style="7" customWidth="1"/>
+    <col min="7" max="7" width="36.85546875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="31.140625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="53.5703125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" style="7" customWidth="1"/>
+    <col min="11" max="11" width="28.5703125" style="7" customWidth="1"/>
+    <col min="12" max="15" width="22.7109375" style="7" customWidth="1"/>
+    <col min="16" max="16" width="30.5703125" style="7" customWidth="1"/>
+    <col min="17" max="105" width="22.7109375" style="7" customWidth="1"/>
+    <col min="106" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:26" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="2:26" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+    </row>
+    <row r="3" spans="2:26" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:26" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="W4" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="2:26" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="H5" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J5" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="K5" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="L5" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="M5" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="N5" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="O5" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="P5" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q5" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="S5" s="7">
+        <v>1</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="U5" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="V5" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="W5" s="20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="2:26" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="I6" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="2:26" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="N7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:26" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="J8" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q8" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="U8" s="18"/>
+    </row>
+    <row r="9" spans="2:26" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="J9" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W9" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="X9" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z9" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="2:26" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="S10" s="7">
+        <v>1</v>
+      </c>
+      <c r="T10" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="U10" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="V10" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="W10" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="X10" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y10" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z10" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="2:26" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+    </row>
+    <row r="12" spans="2:26" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+    </row>
+    <row r="13" spans="2:26" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="U13" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="W13" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="2:26" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="32"/>
+      <c r="F14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="S14" s="7">
+        <v>1</v>
+      </c>
+      <c r="T14" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="U14" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="V14" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="W14" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="2:26" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="E15" s="32"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="S15" s="7">
+        <v>1</v>
+      </c>
+      <c r="T15" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="U15" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="V15" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="W15" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="2:26" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="32"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="S16" s="7">
+        <v>1</v>
+      </c>
+      <c r="T16" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="U16" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="V16" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="W16" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="S17" s="7">
+        <v>1</v>
+      </c>
+      <c r="T17" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="U17" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="V17" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="W17" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+    </row>
+    <row r="19" spans="1:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+    </row>
+    <row r="20" spans="1:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T20" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="23"/>
+      <c r="B21" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="T21" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="U21" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="23"/>
+      <c r="B22" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="T22" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="U22" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+      <c r="T23" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="U23" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="22"/>
+      <c r="T24" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="U24" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="T25" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="U25" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L26" s="13"/>
+      <c r="T26" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="U26" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:D4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="255.5703125" style="7" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
lesson18-database sql ddl & dml p1 - 28.06.2023
</commit_message>
<xml_diff>
--- a/JAVA18 QPHAN DATABASE DESIGN.xlsx
+++ b/JAVA18 QPHAN DATABASE DESIGN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="422" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="422" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="B1. Mô hình quan niệm" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,6 @@
     <sheet name="4. Cơ sở dữ liệu vật lý" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -484,30 +483,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Số lượng còn lại</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="W13" authorId="0" shapeId="0">
       <text>
         <r>
@@ -585,7 +560,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="142">
   <si>
     <t>Xác định các đối tượng cần lưu trữ
 Xác định các thuộc tính, thông tin của từng đối tượng</t>
@@ -913,16 +888,10 @@
     <t>PROVIDER_ID</t>
   </si>
   <si>
-    <t>EMPLOYEE_DETAIL</t>
-  </si>
-  <si>
     <t>EMPLOYEE_ID</t>
   </si>
   <si>
     <t>TITLE_ID</t>
-  </si>
-  <si>
-    <t>Phụ Cấp</t>
   </si>
   <si>
     <t>CUSTOMER_ID</t>
@@ -1183,6 +1152,12 @@
       </rPr>
       <t xml:space="preserve"> Sử dụng TOOL - MySQL workbench</t>
     </r>
+  </si>
+  <si>
+    <t>STIPEND</t>
+  </si>
+  <si>
+    <t>EMPLOYEE_TITLE</t>
   </si>
 </sst>
 </file>
@@ -1428,6 +1403,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1436,9 +1414,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1799,16 +1774,16 @@
       </c>
     </row>
     <row r="2" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
     </row>
     <row r="3" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
       <c r="E3" s="7" t="s">
         <v>5</v>
       </c>
@@ -1817,9 +1792,9 @@
       </c>
     </row>
     <row r="4" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="7" t="s">
         <v>6</v>
       </c>
@@ -2206,8 +2181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V51"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" topLeftCell="M34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T38" sqref="T38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
@@ -2234,16 +2209,16 @@
       </c>
     </row>
     <row r="2" spans="2:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
     </row>
     <row r="3" spans="2:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
       <c r="E3" s="7" t="s">
         <v>5</v>
       </c>
@@ -2252,9 +2227,9 @@
       </c>
     </row>
     <row r="4" spans="2:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="7" t="s">
         <v>6</v>
       </c>
@@ -2789,7 +2764,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="39" t="s">
         <v>57</v>
       </c>
       <c r="B21" s="13" t="s">
@@ -2811,7 +2786,7 @@
       </c>
     </row>
     <row r="22" spans="1:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="38"/>
+      <c r="A22" s="39"/>
       <c r="B22" s="13" t="s">
         <v>51</v>
       </c>
@@ -2945,8 +2920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView topLeftCell="M1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
@@ -2976,18 +2951,18 @@
       </c>
     </row>
     <row r="2" spans="2:26" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
       <c r="E2" s="34"/>
       <c r="F2" s="34"/>
     </row>
     <row r="3" spans="2:26" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
       <c r="E3" s="34"/>
       <c r="F3" s="34"/>
       <c r="G3" s="7" t="s">
@@ -2998,9 +2973,9 @@
       </c>
     </row>
     <row r="4" spans="2:26" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
       <c r="E4" s="34"/>
       <c r="F4" s="34"/>
       <c r="G4" s="7" t="s">
@@ -3029,53 +3004,53 @@
       </c>
     </row>
     <row r="5" spans="2:26" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="F5" s="39" t="s">
+      <c r="F5" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="G5" s="39" t="s">
+      <c r="G5" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="H5" s="39" t="s">
+      <c r="H5" s="36" t="s">
         <v>89</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J5" s="39" t="s">
+      <c r="J5" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="K5" s="39" t="s">
+      <c r="K5" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="L5" s="39" t="s">
+      <c r="L5" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="M5" s="39" t="s">
+      <c r="M5" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="N5" s="39" t="s">
+      <c r="N5" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="O5" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="P5" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="O5" s="39" t="s">
+      <c r="Q5" s="36" t="s">
         <v>120</v>
-      </c>
-      <c r="P5" s="39" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q5" s="39" t="s">
-        <v>122</v>
       </c>
       <c r="S5" s="7">
         <v>1</v>
@@ -3104,7 +3079,7 @@
         <v>24</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>108</v>
+        <v>141</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>32</v>
@@ -3113,10 +3088,10 @@
         <v>35</v>
       </c>
       <c r="H6" s="29" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I6" s="29" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>44</v>
@@ -3154,7 +3129,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F7" s="28" t="s">
         <v>2</v>
@@ -3163,10 +3138,10 @@
         <v>2</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J7" s="28" t="s">
         <v>2</v>
@@ -3204,22 +3179,22 @@
         <v>3</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G8" s="33" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H8" s="30" t="s">
         <v>103</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J8" s="35" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>47</v>
@@ -3265,7 +3240,7 @@
         <v>12</v>
       </c>
       <c r="I9" s="35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J9" s="32" t="s">
         <v>45</v>
@@ -3301,7 +3276,7 @@
         <v>23</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>27</v>
@@ -3311,7 +3286,7 @@
         <v>27</v>
       </c>
       <c r="G10" s="33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3" t="s">
@@ -3325,7 +3300,7 @@
       </c>
       <c r="N10" s="3"/>
       <c r="O10" s="3" t="s">
-        <v>111</v>
+        <v>140</v>
       </c>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
@@ -3388,9 +3363,7 @@
       <c r="B12" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
         <v>29</v>
       </c>
@@ -3491,7 +3464,7 @@
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="33" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E15" s="32"/>
       <c r="F15" s="3"/>
@@ -3796,7 +3769,7 @@
   <dimension ref="A1:A45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
@@ -3807,99 +3780,99 @@
   <sheetData>
     <row r="1" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
lessson18-rdbms sql p2 - 07.05.2023
</commit_message>
<xml_diff>
--- a/JAVA18 QPHAN DATABASE DESIGN.xlsx
+++ b/JAVA18 QPHAN DATABASE DESIGN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="422" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="422" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="B1. Mô hình quan niệm" sheetId="1" r:id="rId1"/>
@@ -430,8 +430,36 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-varchar || char
+INT
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+varchar
+s
+m
+l
+xl</t>
         </r>
       </text>
     </comment>
@@ -560,7 +588,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="147">
   <si>
     <t>Xác định các đối tượng cần lưu trữ
 Xác định các thuộc tính, thông tin của từng đối tượng</t>
@@ -1158,6 +1186,21 @@
   </si>
   <si>
     <t>EMPLOYEE_TITLE</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>Nữ</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
 </sst>
 </file>
@@ -2181,7 +2224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="T38" sqref="T38"/>
     </sheetView>
   </sheetViews>
@@ -2920,8 +2963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z51"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:I10"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
@@ -3069,22 +3112,22 @@
       </c>
     </row>
     <row r="6" spans="2:26" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="29" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="29" t="s">
         <v>141</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="29" t="s">
         <v>35</v>
       </c>
       <c r="H6" s="29" t="s">
@@ -3093,7 +3136,7 @@
       <c r="I6" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="29" t="s">
         <v>44</v>
       </c>
       <c r="K6" s="2" t="s">
@@ -3152,19 +3195,19 @@
       <c r="L7" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="M7" s="16" t="s">
+      <c r="M7" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="N7" s="16" t="s">
+      <c r="N7" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="O7" s="16" t="s">
+      <c r="O7" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="P7" s="16" t="s">
+      <c r="P7" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="Q7" s="16" t="s">
+      <c r="Q7" s="28" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3214,8 +3257,8 @@
       <c r="P8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Q8" s="16" t="s">
-        <v>29</v>
+      <c r="Q8" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="U8" s="18"/>
     </row>
@@ -3256,7 +3299,7 @@
       </c>
       <c r="P9" s="3"/>
       <c r="Q9" s="3" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="W9" s="7" t="s">
         <v>65</v>
@@ -3303,7 +3346,9 @@
         <v>140</v>
       </c>
       <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
+      <c r="Q10" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="S10" s="7">
         <v>1</v>
       </c>
@@ -3619,7 +3664,15 @@
       </c>
       <c r="L21" s="22"/>
       <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
+      <c r="N21" s="22">
+        <v>1</v>
+      </c>
+      <c r="O21" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="P21" s="7" t="s">
+        <v>143</v>
+      </c>
       <c r="T21" s="7" t="s">
         <v>77</v>
       </c>
@@ -3645,7 +3698,15 @@
       </c>
       <c r="L22" s="22"/>
       <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
+      <c r="N22" s="22">
+        <v>2</v>
+      </c>
+      <c r="O22" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="P22" s="7" t="s">
+        <v>144</v>
+      </c>
       <c r="T22" s="7" t="s">
         <v>64</v>
       </c>
@@ -3670,7 +3731,15 @@
       </c>
       <c r="L23" s="22"/>
       <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
+      <c r="N23" s="22">
+        <v>3</v>
+      </c>
+      <c r="O23" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="P23" s="7" t="s">
+        <v>143</v>
+      </c>
       <c r="T23" s="7" t="s">
         <v>69</v>
       </c>
@@ -3693,7 +3762,15 @@
       <c r="K24" s="15"/>
       <c r="L24" s="22"/>
       <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
+      <c r="N24" s="22">
+        <v>4</v>
+      </c>
+      <c r="O24" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="P24" s="7" t="s">
+        <v>144</v>
+      </c>
       <c r="T24" s="7" t="s">
         <v>70</v>
       </c>
@@ -3713,6 +3790,15 @@
       <c r="J25" s="13"/>
       <c r="K25" s="13"/>
       <c r="L25" s="13"/>
+      <c r="N25" s="7">
+        <v>5</v>
+      </c>
+      <c r="O25" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="P25" s="7" t="s">
+        <v>143</v>
+      </c>
       <c r="T25" s="7" t="s">
         <v>71</v>
       </c>
@@ -3722,6 +3808,15 @@
     </row>
     <row r="26" spans="1:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L26" s="13"/>
+      <c r="N26" s="7">
+        <v>6</v>
+      </c>
+      <c r="O26" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="P26" s="7" t="s">
+        <v>144</v>
+      </c>
       <c r="T26" s="7" t="s">
         <v>79</v>
       </c>
@@ -3769,7 +3864,7 @@
   <dimension ref="A1:A45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>

</xml_diff>